<commit_message>
Checkpoint - Coding running well
The code can be optimized to close figures before saving .mat file.
The code can also be automated
</commit_message>
<xml_diff>
--- a/result_manuscriptIII.xlsx
+++ b/result_manuscriptIII.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\ChangValiante2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F060248-49A5-4FB0-97DD-2DF64601A33F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76472638-0EF6-4911-BE33-B252DA6AB119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1898" yWindow="1898" windowWidth="18851" windowHeight="11023" activeTab="1" xr2:uid="{370348AB-59FA-4064-88BB-72F0F661FEE8}"/>
+    <workbookView xWindow="1898" yWindow="1898" windowWidth="18851" windowHeight="11023" activeTab="1" xr2:uid="{47E7848B-34EC-49A6-998D-9AC1D627B3A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="19812000" sheetId="2" r:id="rId2"/>
+    <sheet name="19805000" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,10 +46,10 @@
     <t>AD test, normality</t>
   </si>
   <si>
-    <t>Intensity (mV^2/s), median</t>
-  </si>
-  <si>
-    <t>Intensity (mV^2/s), IQR</t>
+    <t>Power (mV^2/s), median</t>
+  </si>
+  <si>
+    <t>Power (mV^2/s), IQR</t>
   </si>
   <si>
     <t>Light-triggered</t>
@@ -121,10 +121,10 @@
     <t>Group</t>
   </si>
   <si>
-    <t>one-way ANOVA, intensity</t>
-  </si>
-  <si>
-    <t>Multiple Comparison (Tukey-Kramer method), intensity</t>
+    <t>one-way ANOVA, power</t>
+  </si>
+  <si>
+    <t>Multiple Comparison (Tukey-Kramer method), power</t>
   </si>
   <si>
     <t>one-way ANOVA, dominant frequency</t>
@@ -481,7 +481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368ADD51-798A-44B4-B52D-E5ED55FD84F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E24766-3465-4683-8C34-CDF2C4BE43EB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -493,7 +493,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3455638-0F3D-478F-9F24-623DAEA5BA5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF4AE5E-3D36-4E01-8D19-4FE6EE8834FF}">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
@@ -501,10 +501,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -549,37 +545,37 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>25.773408000000018</v>
+        <v>13.349005000000034</v>
       </c>
       <c r="C2">
-        <v>4.6849440000001437</v>
+        <v>5.0429759999997259</v>
       </c>
       <c r="D2">
-        <v>0.10813052312387034</v>
+        <v>0.1346693543526121</v>
       </c>
       <c r="E2">
-        <v>427718.4671063642</v>
+        <v>295335.53033840557</v>
       </c>
       <c r="F2">
-        <v>260160.80614705588</v>
+        <v>154868.4657022437</v>
       </c>
       <c r="G2">
-        <v>6.6579248980920658E-2</v>
+        <v>0.54783149352144311</v>
       </c>
       <c r="H2">
-        <v>2.7279931259552415E-2</v>
+        <v>0.20543240654644268</v>
       </c>
       <c r="I2">
-        <v>15.25927734375</v>
+        <v>12.716064453125</v>
       </c>
       <c r="J2">
-        <v>1.2716064453125</v>
+        <v>10.490753173828125</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-4</v>
+        <v>0.10428483665837576</v>
       </c>
       <c r="L2">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -587,37 +583,28 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>26.859647999999652</v>
+        <v>63.321023999999852</v>
       </c>
       <c r="C3">
-        <v>2.9741279999996095</v>
-      </c>
-      <c r="D3">
-        <v>5.5616357874621707E-2</v>
+        <v>87.460271999999918</v>
       </c>
       <c r="E3">
-        <v>414085.68714779901</v>
+        <v>130799.00983475964</v>
       </c>
       <c r="F3">
-        <v>125928.80908454815</v>
-      </c>
-      <c r="G3">
-        <v>0.5797927609451361</v>
+        <v>116988.38552699925</v>
       </c>
       <c r="H3">
-        <v>5.6066262743570405E-14</v>
+        <v>7.1529707079602822E-3</v>
       </c>
       <c r="I3">
-        <v>16.212982177734375</v>
+        <v>16.848785400390625</v>
       </c>
       <c r="J3">
-        <v>7.8680648803710938</v>
-      </c>
-      <c r="K3">
-        <v>6.5940482305243589E-2</v>
+        <v>5.72222900390625</v>
       </c>
       <c r="L3">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -625,37 +612,37 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>24.66172799999913</v>
+        <v>21.63110400000005</v>
       </c>
       <c r="C4">
-        <v>5.5079279999995379</v>
+        <v>3.5627520000005006</v>
       </c>
       <c r="D4">
-        <v>0.3606006889232749</v>
+        <v>0.85073937132171151</v>
       </c>
       <c r="E4">
-        <v>295410.47548677668</v>
+        <v>69455.789809561044</v>
       </c>
       <c r="F4">
-        <v>72611.511211585486</v>
+        <v>4907.3794468311535</v>
       </c>
       <c r="G4">
-        <v>0.38094228659085061</v>
+        <v>0.61070674819712234</v>
       </c>
       <c r="H4">
-        <v>1.3946154254762533E-6</v>
+        <v>7.8273477437384997E-4</v>
       </c>
       <c r="I4">
-        <v>18.120391845703125</v>
+        <v>10.80865478515625</v>
       </c>
       <c r="J4">
-        <v>6.1196060180664063</v>
+        <v>2.3842620849609375</v>
       </c>
       <c r="K4">
-        <v>0.97235305289678287</v>
+        <v>0.14941531559866775</v>
       </c>
       <c r="L4">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -692,31 +679,31 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>8.0646472513673989E-2</v>
+        <v>4.0271940537589179E-3</v>
       </c>
       <c r="C6">
-        <v>0.33069828722002637</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>-0.35177865612648224</v>
+        <v>-1</v>
       </c>
       <c r="E6">
-        <v>0.14135208910397801</v>
+        <v>0.15369438002288383</v>
       </c>
       <c r="F6">
-        <v>0.30039525691699598</v>
+        <v>0.64285714285714279</v>
       </c>
       <c r="G6">
-        <v>0.10935441370223979</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I6">
-        <v>0.14803906926700378</v>
+        <v>0.61866473176178638</v>
       </c>
       <c r="J6">
-        <v>0.29776021080368908</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="K6">
-        <v>4.4795783926218712E-2</v>
+        <v>-0.45238095238095238</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -749,19 +736,19 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>54.925018084178589</v>
+        <v>14305.845705040392</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>27.462509042089295</v>
+        <v>7152.9228525201961</v>
       </c>
       <c r="E10">
-        <v>2.2354627187389444</v>
+        <v>16.508662104615993</v>
       </c>
       <c r="F10">
-        <v>0.11522874717500298</v>
+        <v>6.9944429386484559E-5</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -769,13 +756,13 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>786.23569248571584</v>
+        <v>8232.3772415139028</v>
       </c>
       <c r="C11">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D11">
-        <v>12.28493269508931</v>
+        <v>433.28301271125804</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -783,10 +770,10 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>841.16071056989449</v>
+        <v>22538.222946554295</v>
       </c>
       <c r="C12">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -813,16 +800,16 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>-4.2402331190250635</v>
+        <v>-109.43190018609994</v>
       </c>
       <c r="D16">
-        <v>-1.9558632727274237</v>
+        <v>-75.788774857142613</v>
       </c>
       <c r="E16">
-        <v>0.32850657357021573</v>
+        <v>-42.145649528185281</v>
       </c>
       <c r="F16">
-        <v>0.10768796909335021</v>
+        <v>4.639545227236308E-5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -833,16 +820,16 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>-3.657029026898162</v>
+        <v>-35.470401833081965</v>
       </c>
       <c r="D17">
-        <v>-0.57403636363613941</v>
+        <v>-7.920230857142764</v>
       </c>
       <c r="E17">
-        <v>2.5089562996258832</v>
+        <v>19.629940118796441</v>
       </c>
       <c r="F17">
-        <v>0.89600813382789601</v>
+        <v>0.74880708738790736</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -853,16 +840,16 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>-1.546141043962014</v>
+        <v>29.250001246734406</v>
       </c>
       <c r="D18">
-        <v>1.3818269090912843</v>
+        <v>67.868543999999844</v>
       </c>
       <c r="E18">
-        <v>4.3097948621445825</v>
+        <v>106.48708675326529</v>
       </c>
       <c r="F18">
-        <v>0.49787264177296109</v>
+        <v>7.4209148172221795E-4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -895,19 +882,19 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>125715924169.00975</v>
+        <v>197212821663.99551</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>62857962084.504875</v>
+        <v>98606410831.997757</v>
       </c>
       <c r="E22">
-        <v>4.9369436035761352</v>
+        <v>13.436592208563308</v>
       </c>
       <c r="F22">
-        <v>1.0140250974827073E-2</v>
+        <v>2.3086057016801487E-4</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,13 +902,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>814858320539.5072</v>
+        <v>139434298274.97025</v>
       </c>
       <c r="C23">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>12732161258.4298</v>
+        <v>7338647277.6300125</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -929,10 +916,10 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>940574244708.51697</v>
+        <v>336647119938.96576</v>
       </c>
       <c r="C24">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -959,16 +946,16 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>-75891.991755188617</v>
+        <v>-10407.900417154189</v>
       </c>
       <c r="D28">
-        <v>-2350.727201330883</v>
+        <v>128050.24477535408</v>
       </c>
       <c r="E28">
-        <v>71190.537352526851</v>
+        <v>266508.38996786234</v>
       </c>
       <c r="F28">
-        <v>0.99676231003021887</v>
+        <v>7.2881588095692007E-2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -979,16 +966,16 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>16262.765931619622</v>
+        <v>110605.65395859678</v>
       </c>
       <c r="D29">
-        <v>115514.28574747598</v>
+        <v>223988.2703406057</v>
       </c>
       <c r="E29">
-        <v>214765.80556333234</v>
+        <v>337370.88672261464</v>
       </c>
       <c r="F29">
-        <v>1.8636887928825008E-2</v>
+        <v>2.1553413097430418E-4</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -999,16 +986,16 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>23604.240688265389</v>
+        <v>-62996.429761715175</v>
       </c>
       <c r="D30">
-        <v>117865.01294880686</v>
+        <v>95938.025565251621</v>
       </c>
       <c r="E30">
-        <v>212125.78520934834</v>
+        <v>254872.48089221842</v>
       </c>
       <c r="F30">
-        <v>1.0585488305823954E-2</v>
+        <v>0.29819585477497634</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1041,19 +1028,19 @@
         <v>24</v>
       </c>
       <c r="B34">
-        <v>9.1919859062820652</v>
+        <v>68.465184405113433</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>4.5959929531410326</v>
+        <v>34.232592202556717</v>
       </c>
       <c r="E34">
-        <v>0.16710166373383514</v>
+        <v>1.1948483361643591</v>
       </c>
       <c r="F34">
-        <v>0.84648154402203524</v>
+        <v>0.32450041998049328</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1061,13 +1048,13 @@
         <v>25</v>
       </c>
       <c r="B35">
-        <v>1760.2670280383761</v>
+        <v>544.35297950576728</v>
       </c>
       <c r="C35">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D35">
-        <v>27.504172313099627</v>
+        <v>28.650156816093016</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1075,10 +1062,10 @@
         <v>26</v>
       </c>
       <c r="B36">
-        <v>1769.4590139446582</v>
+        <v>612.81816391088068</v>
       </c>
       <c r="C36">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1105,16 +1092,16 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>-2.6394285526846715</v>
+        <v>-13.669457229189122</v>
       </c>
       <c r="D40">
-        <v>0.77862858426743387</v>
+        <v>-5.018304007393974</v>
       </c>
       <c r="E40">
-        <v>4.1966857212195396</v>
+        <v>3.6328492144011744</v>
       </c>
       <c r="F40">
-        <v>0.84858559197877992</v>
+        <v>0.32530873961456097</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1125,16 +1112,16 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>-4.4798285841480645</v>
+        <v>-6.6983585819798455</v>
       </c>
       <c r="D41">
-        <v>0.13319197944972672</v>
+        <v>0.38602338518415102</v>
       </c>
       <c r="E41">
-        <v>4.7462125430475179</v>
+        <v>7.4704053523481475</v>
       </c>
       <c r="F41">
-        <v>0.99735751222979241</v>
+        <v>0.989497227549061</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1145,16 +1132,16 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>-5.0264967798682312</v>
+        <v>-4.5262283240569037</v>
       </c>
       <c r="D42">
-        <v>-0.64543660481770715</v>
+        <v>5.404327392578125</v>
       </c>
       <c r="E42">
-        <v>3.7356235702328169</v>
+        <v>15.334883109213154</v>
       </c>
       <c r="F42">
-        <v>0.93351335239121924</v>
+        <v>0.36948258883147278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>